<commit_message>
Repaired ESS1 and PV1 relay settings.
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/DER_relay.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/DER_relay.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="7008" windowWidth="23256" windowHeight="2340"/>
+    <workbookView xWindow="-15" yWindow="7005" windowWidth="19440" windowHeight="2340"/>
   </bookViews>
   <sheets>
     <sheet name="relays" sheetId="1" r:id="rId1"/>
@@ -775,29 +775,29 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.109375" style="6" customWidth="1"/>
+    <col min="1" max="2" width="11.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="6" customWidth="1"/>
-    <col min="12" max="15" width="12.5546875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="17.33203125" style="6" customWidth="1"/>
-    <col min="19" max="20" width="12.5546875" style="6" customWidth="1"/>
-    <col min="21" max="21" width="11.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="6" customWidth="1"/>
+    <col min="12" max="15" width="12.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="6" customWidth="1"/>
+    <col min="19" max="20" width="12.5703125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" style="6" customWidth="1"/>
     <col min="22" max="22" width="12" style="6" customWidth="1"/>
-    <col min="23" max="16384" width="9.109375" style="6"/>
+    <col min="23" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -936,15 +936,15 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <v>13800</v>
+        <v>480</v>
       </c>
       <c r="C3" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5">
         <v>12</v>
@@ -956,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="12">
-        <v>1200</v>
+        <v>3500</v>
       </c>
       <c r="H3" s="11">
         <v>0</v>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="13">
-        <v>0.60140653040586012</v>
+        <v>1</v>
       </c>
       <c r="L3" s="6">
         <v>1</v>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="13">
-        <v>0.60140653040586012</v>
+        <v>0.40093768693724008</v>
       </c>
       <c r="S3" s="6">
         <v>1</v>
@@ -1004,15 +1004,15 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="6">
-        <v>13800</v>
+        <v>480</v>
       </c>
       <c r="C4" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" s="5">
         <v>12</v>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="12">
-        <v>1200</v>
+        <v>3500</v>
       </c>
       <c r="H4" s="11">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="13">
-        <v>0.60140653040586012</v>
+        <v>2</v>
       </c>
       <c r="L4" s="6">
         <v>1</v>
@@ -1057,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="13">
-        <v>0.60140653040586012</v>
+        <v>0.40093768693724008</v>
       </c>
       <c r="S4" s="6">
         <v>1</v>
@@ -1072,7 +1072,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="D9" s="9"/>
@@ -1355,7 +1355,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="D10" s="9"/>
@@ -1366,7 +1366,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="D11" s="9"/>
@@ -1377,7 +1377,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="D12" s="9"/>
@@ -1388,7 +1388,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="D13" s="9"/>

</xml_diff>

<commit_message>
Added 81/81rf protections configs to xls protective relay config
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/DER_relay.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/DER_relay.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="7005" windowWidth="19440" windowHeight="2340"/>
+    <workbookView xWindow="-12" yWindow="7008" windowWidth="19440" windowHeight="2340"/>
   </bookViews>
   <sheets>
     <sheet name="relays" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>VRMSLL</t>
   </si>
@@ -59,6 +59,29 @@
   </si>
   <si>
     <t>CB Initial State [closed=1; open=0]</t>
+  </si>
+  <si>
+    <t>81U Trip Pickup [Hz]</t>
+  </si>
+  <si>
+    <t>81U Trip Delay [Sec]</t>
+  </si>
+  <si>
+    <t>81O Trip Pickup [Hz]</t>
+  </si>
+  <si>
+    <t>81O Trip Delay [Sec]</t>
+  </si>
+  <si>
+    <t>81RFRP
+[Hz/Sec]</t>
+  </si>
+  <si>
+    <t>81RFDFP
+[Hz]</t>
+  </si>
+  <si>
+    <t>81RF Trip Delay [Sec]</t>
   </si>
 </sst>
 </file>
@@ -482,6 +505,44 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>533682</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>137383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17160240" y="2324100"/>
+          <a:ext cx="3254022" cy="2568163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -772,35 +833,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.140625" style="6" customWidth="1"/>
+    <col min="1" max="2" width="11.109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="6" customWidth="1"/>
-    <col min="12" max="15" width="12.5703125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" style="6" customWidth="1"/>
-    <col min="19" max="20" width="12.5703125" style="6" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" style="6" customWidth="1"/>
-    <col min="22" max="22" width="12" style="6" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="14.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" style="6" customWidth="1"/>
+    <col min="12" max="15" width="12.5546875" style="6" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="13" style="6" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="6" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" style="6" customWidth="1"/>
+    <col min="20" max="21" width="9.109375" style="6"/>
+    <col min="22" max="22" width="11.109375" style="6" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" style="6" customWidth="1"/>
+    <col min="24" max="24" width="12.5546875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="6" customWidth="1"/>
+    <col min="26" max="27" width="12.5546875" style="6" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" style="6" customWidth="1"/>
+    <col min="29" max="29" width="12" style="6" customWidth="1"/>
+    <col min="30" max="30" width="13.44140625" style="6" customWidth="1"/>
+    <col min="31" max="31" width="13" style="6" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" style="6" customWidth="1"/>
+    <col min="33" max="33" width="12.109375" style="6" customWidth="1"/>
+    <col min="34" max="35" width="9.109375" style="6"/>
+    <col min="36" max="36" width="11.109375" style="6" customWidth="1"/>
+    <col min="37" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -846,29 +919,71 @@
       <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="AD1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -915,28 +1030,70 @@
         <v>1.2</v>
       </c>
       <c r="P2" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>2</v>
+      </c>
+      <c r="R2" s="6">
+        <v>66</v>
+      </c>
+      <c r="S2" s="6">
+        <v>2</v>
+      </c>
+      <c r="T2" s="6">
+        <v>2</v>
+      </c>
+      <c r="U2" s="6">
+        <v>57</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W2" s="6">
         <v>20</v>
       </c>
-      <c r="Q2" s="6">
-        <v>0</v>
-      </c>
-      <c r="R2" s="13">
+      <c r="X2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="13">
         <v>0.60140653040586012</v>
       </c>
-      <c r="S2" s="6">
-        <v>1</v>
-      </c>
-      <c r="T2" s="6">
-        <v>1</v>
-      </c>
-      <c r="U2" s="6">
+      <c r="Z2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="6">
         <v>0.5</v>
       </c>
-      <c r="V2" s="6">
+      <c r="AC2" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD2" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -983,28 +1140,70 @@
         <v>1.2</v>
       </c>
       <c r="P3" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>2</v>
+      </c>
+      <c r="R3" s="6">
+        <v>66</v>
+      </c>
+      <c r="S3" s="6">
+        <v>2</v>
+      </c>
+      <c r="T3" s="6">
+        <v>2</v>
+      </c>
+      <c r="U3" s="6">
+        <v>57</v>
+      </c>
+      <c r="V3" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W3" s="6">
         <v>20</v>
       </c>
-      <c r="Q3" s="6">
-        <v>0</v>
-      </c>
-      <c r="R3" s="13">
+      <c r="X3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="13">
         <v>0.40093768693724008</v>
       </c>
-      <c r="S3" s="6">
-        <v>1</v>
-      </c>
-      <c r="T3" s="6">
-        <v>1</v>
-      </c>
-      <c r="U3" s="6">
+      <c r="Z3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="6">
         <v>0.5</v>
       </c>
-      <c r="V3" s="6">
+      <c r="AC3" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD3" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE3" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG3" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ3" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1051,28 +1250,70 @@
         <v>1.2</v>
       </c>
       <c r="P4" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>2</v>
+      </c>
+      <c r="R4" s="6">
+        <v>66</v>
+      </c>
+      <c r="S4" s="6">
+        <v>2</v>
+      </c>
+      <c r="T4" s="6">
+        <v>2</v>
+      </c>
+      <c r="U4" s="6">
+        <v>57</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W4" s="6">
         <v>20</v>
       </c>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-      <c r="R4" s="13">
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="13">
         <v>0.40093768693724008</v>
       </c>
-      <c r="S4" s="6">
-        <v>1</v>
-      </c>
-      <c r="T4" s="6">
-        <v>1</v>
-      </c>
-      <c r="U4" s="6">
+      <c r="Z4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="6">
         <v>0.5</v>
       </c>
-      <c r="V4" s="6">
+      <c r="AC4" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD4" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG4" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1119,28 +1360,70 @@
         <v>1.2</v>
       </c>
       <c r="P5" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>2</v>
+      </c>
+      <c r="R5" s="6">
+        <v>66</v>
+      </c>
+      <c r="S5" s="6">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6">
+        <v>2</v>
+      </c>
+      <c r="U5" s="6">
+        <v>57</v>
+      </c>
+      <c r="V5" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W5" s="6">
         <v>20</v>
       </c>
-      <c r="Q5" s="6">
-        <v>0</v>
-      </c>
-      <c r="R5" s="13">
+      <c r="X5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="13">
         <v>0.60140653040586012</v>
       </c>
-      <c r="S5" s="6">
-        <v>1</v>
-      </c>
-      <c r="T5" s="6">
-        <v>1</v>
-      </c>
-      <c r="U5" s="6">
+      <c r="Z5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="6">
         <v>0.5</v>
       </c>
-      <c r="V5" s="6">
+      <c r="AC5" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD5" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE5" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG5" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1187,28 +1470,70 @@
         <v>1.2</v>
       </c>
       <c r="P6" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>2</v>
+      </c>
+      <c r="R6" s="6">
+        <v>66</v>
+      </c>
+      <c r="S6" s="6">
+        <v>2</v>
+      </c>
+      <c r="T6" s="6">
+        <v>2</v>
+      </c>
+      <c r="U6" s="6">
+        <v>57</v>
+      </c>
+      <c r="V6" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W6" s="6">
         <v>20</v>
       </c>
-      <c r="Q6" s="6">
-        <v>0</v>
-      </c>
-      <c r="R6" s="13">
+      <c r="X6" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="13">
         <v>0.40093768693724008</v>
       </c>
-      <c r="S6" s="6">
-        <v>1</v>
-      </c>
-      <c r="T6" s="6">
-        <v>1</v>
-      </c>
-      <c r="U6" s="6">
+      <c r="Z6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="6">
         <v>0.5</v>
       </c>
-      <c r="V6" s="6">
+      <c r="AC6" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD6" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE6" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG6" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1255,28 +1580,70 @@
         <v>1.2</v>
       </c>
       <c r="P7" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>2</v>
+      </c>
+      <c r="R7" s="6">
+        <v>66</v>
+      </c>
+      <c r="S7" s="6">
+        <v>2</v>
+      </c>
+      <c r="T7" s="6">
+        <v>2</v>
+      </c>
+      <c r="U7" s="6">
+        <v>57</v>
+      </c>
+      <c r="V7" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W7" s="6">
         <v>20</v>
       </c>
-      <c r="Q7" s="6">
-        <v>0</v>
-      </c>
-      <c r="R7" s="13">
+      <c r="X7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="13">
         <v>0.40093768693724008</v>
       </c>
-      <c r="S7" s="6">
-        <v>1</v>
-      </c>
-      <c r="T7" s="6">
-        <v>1</v>
-      </c>
-      <c r="U7" s="6">
+      <c r="Z7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="6">
         <v>0.5</v>
       </c>
-      <c r="V7" s="6">
+      <c r="AC7" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD7" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ7" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1323,28 +1690,70 @@
         <v>1.2</v>
       </c>
       <c r="P8" s="6">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>2</v>
+      </c>
+      <c r="R8" s="6">
+        <v>66</v>
+      </c>
+      <c r="S8" s="6">
+        <v>2</v>
+      </c>
+      <c r="T8" s="6">
+        <v>2</v>
+      </c>
+      <c r="U8" s="6">
+        <v>57</v>
+      </c>
+      <c r="V8" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W8" s="6">
         <v>20</v>
       </c>
-      <c r="Q8" s="6">
-        <v>0</v>
-      </c>
-      <c r="R8" s="13">
+      <c r="X8" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="13">
         <v>1.1856300170858387</v>
       </c>
-      <c r="S8" s="6">
-        <v>1</v>
-      </c>
-      <c r="T8" s="6">
-        <v>1</v>
-      </c>
-      <c r="U8" s="6">
+      <c r="Z8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="6">
         <v>0.5</v>
       </c>
-      <c r="V8" s="6">
+      <c r="AC8" s="6">
         <v>1.2</v>
       </c>
+      <c r="AD8" s="6">
+        <v>54</v>
+      </c>
+      <c r="AE8" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="6">
+        <v>66</v>
+      </c>
+      <c r="AG8" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="6">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ8" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="D9" s="9"/>
@@ -1355,7 +1764,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="D10" s="9"/>
@@ -1366,7 +1775,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="D11" s="9"/>
@@ -1377,7 +1786,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="D12" s="9"/>
@@ -1388,7 +1797,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="D13" s="9"/>

</xml_diff>

<commit_message>
Fixed issues with 81RF protective element Changed default xls parameters to disable 81x protections. Added goose messages for DER's cb's
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/DER_relay.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/DER_relay.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="7008" windowWidth="19440" windowHeight="2340"/>
+    <workbookView xWindow="-15" yWindow="7005" windowWidth="19440" windowHeight="2340"/>
   </bookViews>
   <sheets>
     <sheet name="relays" sheetId="1" r:id="rId1"/>
@@ -835,45 +835,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2:AJ8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.109375" style="6" customWidth="1"/>
+    <col min="1" max="2" width="11.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="6" customWidth="1"/>
-    <col min="12" max="15" width="12.5546875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="6" customWidth="1"/>
+    <col min="12" max="15" width="12.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" style="6" customWidth="1"/>
     <col min="17" max="17" width="13" style="6" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="12.109375" style="6" customWidth="1"/>
-    <col min="20" max="21" width="9.109375" style="6"/>
-    <col min="22" max="22" width="11.109375" style="6" customWidth="1"/>
-    <col min="23" max="23" width="17.33203125" style="6" customWidth="1"/>
-    <col min="24" max="24" width="12.5546875" style="6" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="6" customWidth="1"/>
-    <col min="26" max="27" width="12.5546875" style="6" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="6" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" style="6" customWidth="1"/>
+    <col min="20" max="21" width="9.140625" style="6"/>
+    <col min="22" max="22" width="11.140625" style="6" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" style="6" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" style="6" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" style="6" customWidth="1"/>
+    <col min="26" max="27" width="12.5703125" style="6" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" style="6" customWidth="1"/>
     <col min="29" max="29" width="12" style="6" customWidth="1"/>
-    <col min="30" max="30" width="13.44140625" style="6" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" style="6" customWidth="1"/>
     <col min="31" max="31" width="13" style="6" customWidth="1"/>
-    <col min="32" max="32" width="11.6640625" style="6" customWidth="1"/>
-    <col min="33" max="33" width="12.109375" style="6" customWidth="1"/>
-    <col min="34" max="35" width="9.109375" style="6"/>
-    <col min="36" max="36" width="11.109375" style="6" customWidth="1"/>
-    <col min="37" max="16384" width="9.109375" style="6"/>
+    <col min="32" max="32" width="11.7109375" style="6" customWidth="1"/>
+    <col min="33" max="33" width="12.140625" style="6" customWidth="1"/>
+    <col min="34" max="35" width="9.140625" style="6"/>
+    <col min="36" max="36" width="11.140625" style="6" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" s="7" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -983,7 +983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1042,13 +1042,13 @@
         <v>2</v>
       </c>
       <c r="T2" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U2" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V2" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W2" s="6">
         <v>20</v>
@@ -1084,16 +1084,16 @@
         <v>2</v>
       </c>
       <c r="AH2" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI2" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ2" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1152,13 +1152,13 @@
         <v>2</v>
       </c>
       <c r="T3" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U3" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V3" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W3" s="6">
         <v>20</v>
@@ -1194,16 +1194,16 @@
         <v>2</v>
       </c>
       <c r="AH3" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI3" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ3" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1262,13 +1262,13 @@
         <v>2</v>
       </c>
       <c r="T4" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U4" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V4" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W4" s="6">
         <v>20</v>
@@ -1304,16 +1304,16 @@
         <v>2</v>
       </c>
       <c r="AH4" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI4" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ4" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1372,13 +1372,13 @@
         <v>2</v>
       </c>
       <c r="T5" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U5" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V5" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W5" s="6">
         <v>20</v>
@@ -1414,16 +1414,16 @@
         <v>2</v>
       </c>
       <c r="AH5" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI5" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ5" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1482,13 +1482,13 @@
         <v>2</v>
       </c>
       <c r="T6" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U6" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V6" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W6" s="6">
         <v>20</v>
@@ -1524,16 +1524,16 @@
         <v>2</v>
       </c>
       <c r="AH6" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI6" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ6" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1592,13 +1592,13 @@
         <v>2</v>
       </c>
       <c r="T7" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U7" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V7" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W7" s="6">
         <v>20</v>
@@ -1634,16 +1634,16 @@
         <v>2</v>
       </c>
       <c r="AH7" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI7" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ7" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1702,13 +1702,13 @@
         <v>2</v>
       </c>
       <c r="T8" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="U8" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V8" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W8" s="6">
         <v>20</v>
@@ -1744,16 +1744,16 @@
         <v>2</v>
       </c>
       <c r="AH8" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="AI8" s="6">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="AJ8" s="6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="D9" s="9"/>
@@ -1764,7 +1764,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="D10" s="9"/>
@@ -1775,7 +1775,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="D11" s="9"/>
@@ -1786,7 +1786,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="D12" s="9"/>
@@ -1797,7 +1797,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="D13" s="9"/>

</xml_diff>